<commit_message>
More Employment Script Updates
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2015/Employment/ACS 2013-2017 Incommute by Industry.xlsx
+++ b/applications/travel_model_lu_inputs/2015/Employment/ACS 2013-2017 Incommute by Industry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11633" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11633" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="8" r:id="rId1"/>
@@ -2083,10 +2083,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10764,8 +10765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10774,7 +10775,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>510</v>
       </c>
     </row>
@@ -10808,25 +10809,25 @@
       <c r="A3" t="s">
         <v>427</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2635</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>148656</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>264684</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>147552</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>92711</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>70309</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>726547</v>
       </c>
     </row>
@@ -10834,25 +10835,25 @@
       <c r="A4" t="s">
         <v>429</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3911</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>95133</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>146907</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>50322</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>49299</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>42981</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>388553</v>
       </c>
     </row>
@@ -10860,25 +10861,25 @@
       <c r="A5" t="s">
         <v>431</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>954</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>32060</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>49589</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>12238</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>18746</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>14024</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>127611</v>
       </c>
     </row>
@@ -10886,25 +10887,25 @@
       <c r="A6" t="s">
         <v>433</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5200</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>10276</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>30656</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>14706</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>8068</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>7709</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>76615</v>
       </c>
     </row>
@@ -10912,25 +10913,25 @@
       <c r="A7" t="s">
         <v>435</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1573</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>236585</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>238502</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>71194</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>105521</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>62360</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>715735</v>
       </c>
     </row>
@@ -10938,25 +10939,25 @@
       <c r="A8" t="s">
         <v>437</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>2282</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>109021</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>120804</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>75868</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>53430</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>38850</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>400255</v>
       </c>
     </row>
@@ -10964,25 +10965,25 @@
       <c r="A9" t="s">
         <v>439</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>5818</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>263972</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>320817</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>237602</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>146189</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>93460</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>1067858</v>
       </c>
     </row>
@@ -10990,25 +10991,25 @@
       <c r="A10" t="s">
         <v>441</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>2332</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>20021</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>56536</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>23392</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>26955</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>17783</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>147019</v>
       </c>
     </row>
@@ -11016,25 +11017,25 @@
       <c r="A11" t="s">
         <v>443</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>7095</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>38801</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>85397</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>38321</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>30066</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>27079</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>226759</v>
       </c>
     </row>
@@ -11042,25 +11043,25 @@
       <c r="A12" t="s">
         <v>444</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>31800</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>954525</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>1313892</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>671195</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>530985</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>374555</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>3876952</v>
       </c>
     </row>
@@ -11095,7 +11096,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>509</v>
       </c>
     </row>
@@ -11129,25 +11130,25 @@
       <c r="A17" t="s">
         <v>498</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>1921</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>138309</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>253802</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>131092</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>81870</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>66171</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <f>SUM(B17:G17)</f>
         <v>673165</v>
       </c>
@@ -11156,25 +11157,25 @@
       <c r="A18" t="s">
         <v>499</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>3259</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>91077</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>144562</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>47394</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>44507</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>42611</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <f t="shared" ref="H18:H26" si="1">SUM(B18:G18)</f>
         <v>373410</v>
       </c>
@@ -11183,25 +11184,25 @@
       <c r="A19" t="s">
         <v>500</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>888</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>32394</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>48116</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>11954</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>16997</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>14189</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <f t="shared" si="1"/>
         <v>124538</v>
       </c>
@@ -11210,25 +11211,25 @@
       <c r="A20" t="s">
         <v>501</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>4762</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>9476</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>29663</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>13787</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>7986</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>7345</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <f t="shared" si="1"/>
         <v>73019</v>
       </c>
@@ -11237,25 +11238,25 @@
       <c r="A21" t="s">
         <v>502</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>1677</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>232852</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>234628</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>65954</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>101827</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>60457</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <f t="shared" si="1"/>
         <v>697395</v>
       </c>
@@ -11264,25 +11265,25 @@
       <c r="A22" t="s">
         <v>503</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>2126</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>104655</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>118645</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>70556</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>49878</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>37641</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <f t="shared" si="1"/>
         <v>383501</v>
       </c>
@@ -11291,25 +11292,25 @@
       <c r="A23" t="s">
         <v>504</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>4944</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>249554</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>305609</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>218765</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>130364</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>86989</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <f t="shared" si="1"/>
         <v>996225</v>
       </c>
@@ -11318,25 +11319,25 @@
       <c r="A24" t="s">
         <v>505</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>1813</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>19506</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>51650</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>19273</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>22223</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>16252</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <f t="shared" si="1"/>
         <v>130717</v>
       </c>
@@ -11345,25 +11346,25 @@
       <c r="A25" t="s">
         <v>506</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>6176</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>37662</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>86231</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>37276</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>27926</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>26515</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <f t="shared" si="1"/>
         <v>221786</v>
       </c>
@@ -11372,31 +11373,31 @@
       <c r="A26" t="s">
         <v>444</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <f>SUM(B17:B25)</f>
         <v>27566</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <f t="shared" ref="C26:G26" si="2">SUM(C17:C25)</f>
         <v>915485</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <f t="shared" si="2"/>
         <v>1272906</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <f t="shared" si="2"/>
         <v>616051</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <f t="shared" si="2"/>
         <v>483578</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <f t="shared" si="2"/>
         <v>358170</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <f t="shared" si="1"/>
         <v>3673756</v>
       </c>
@@ -11441,7 +11442,7 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>511</v>
       </c>
     </row>
@@ -11475,31 +11476,31 @@
       <c r="A31" t="s">
         <v>498</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <f t="shared" ref="B31:B40" si="9">B3-B17</f>
         <v>714</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <f t="shared" ref="C31:H31" si="10">C3-C17</f>
         <v>10347</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <f t="shared" si="10"/>
         <v>10882</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <f t="shared" si="10"/>
         <v>16460</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <f t="shared" si="10"/>
         <v>10841</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <f t="shared" si="10"/>
         <v>4138</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <f t="shared" si="10"/>
         <v>53382</v>
       </c>
@@ -11508,31 +11509,31 @@
       <c r="A32" t="s">
         <v>499</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <f t="shared" si="9"/>
         <v>652</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <f t="shared" ref="C32:H40" si="11">C4-C18</f>
         <v>4056</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <f t="shared" si="11"/>
         <v>2345</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <f t="shared" si="11"/>
         <v>2928</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <f t="shared" si="11"/>
         <v>4792</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <f t="shared" si="11"/>
         <v>370</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <f t="shared" si="11"/>
         <v>15143</v>
       </c>
@@ -11541,31 +11542,31 @@
       <c r="A33" t="s">
         <v>500</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <f t="shared" si="9"/>
         <v>66</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <f t="shared" si="11"/>
         <v>-334</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <f t="shared" si="11"/>
         <v>1473</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <f t="shared" si="11"/>
         <v>284</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <f t="shared" si="11"/>
         <v>1749</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <f t="shared" si="11"/>
         <v>-165</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <f t="shared" si="11"/>
         <v>3073</v>
       </c>
@@ -11574,31 +11575,31 @@
       <c r="A34" t="s">
         <v>501</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <f t="shared" si="9"/>
         <v>438</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <f t="shared" si="11"/>
         <v>800</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <f t="shared" si="11"/>
         <v>993</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <f t="shared" si="11"/>
         <v>919</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <f t="shared" si="11"/>
         <v>82</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <f t="shared" si="11"/>
         <v>364</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <f t="shared" si="11"/>
         <v>3596</v>
       </c>
@@ -11607,31 +11608,31 @@
       <c r="A35" t="s">
         <v>502</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <f t="shared" si="9"/>
         <v>-104</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <f t="shared" si="11"/>
         <v>3733</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <f t="shared" si="11"/>
         <v>3874</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <f t="shared" si="11"/>
         <v>5240</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <f t="shared" si="11"/>
         <v>3694</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2">
         <f t="shared" si="11"/>
         <v>1903</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="2">
         <f t="shared" si="11"/>
         <v>18340</v>
       </c>
@@ -11640,31 +11641,31 @@
       <c r="A36" t="s">
         <v>503</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <f t="shared" si="9"/>
         <v>156</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <f t="shared" si="11"/>
         <v>4366</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <f t="shared" si="11"/>
         <v>2159</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <f t="shared" si="11"/>
         <v>5312</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <f t="shared" si="11"/>
         <v>3552</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <f t="shared" si="11"/>
         <v>1209</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <f t="shared" si="11"/>
         <v>16754</v>
       </c>
@@ -11673,31 +11674,31 @@
       <c r="A37" t="s">
         <v>504</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <f t="shared" si="9"/>
         <v>874</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <f t="shared" si="11"/>
         <v>14418</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <f t="shared" si="11"/>
         <v>15208</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <f t="shared" si="11"/>
         <v>18837</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <f t="shared" si="11"/>
         <v>15825</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2">
         <f t="shared" si="11"/>
         <v>6471</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="2">
         <f t="shared" si="11"/>
         <v>71633</v>
       </c>
@@ -11706,31 +11707,31 @@
       <c r="A38" t="s">
         <v>505</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <f t="shared" si="9"/>
         <v>519</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <f t="shared" si="11"/>
         <v>515</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <f t="shared" si="11"/>
         <v>4886</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <f t="shared" si="11"/>
         <v>4119</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <f t="shared" si="11"/>
         <v>4732</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <f t="shared" si="11"/>
         <v>1531</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <f t="shared" si="11"/>
         <v>16302</v>
       </c>
@@ -11739,31 +11740,31 @@
       <c r="A39" t="s">
         <v>506</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <f t="shared" si="9"/>
         <v>919</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <f t="shared" si="11"/>
         <v>1139</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <f t="shared" si="11"/>
         <v>-834</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <f t="shared" si="11"/>
         <v>1045</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <f t="shared" si="11"/>
         <v>2140</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <f t="shared" si="11"/>
         <v>564</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="2">
         <f t="shared" si="11"/>
         <v>4973</v>
       </c>
@@ -11772,31 +11773,31 @@
       <c r="A40" t="s">
         <v>444</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <f t="shared" si="9"/>
         <v>4234</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <f t="shared" si="11"/>
         <v>39040</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <f t="shared" si="11"/>
         <v>40986</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <f t="shared" si="11"/>
         <v>55144</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <f t="shared" si="11"/>
         <v>47407</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <f t="shared" si="11"/>
         <v>16385</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <f t="shared" si="11"/>
         <v>203196</v>
       </c>
@@ -11844,7 +11845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tidy up ESRI employment script
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2015/Employment/ACS 2013-2017 Incommute by Industry.xlsx
+++ b/applications/travel_model_lu_inputs/2015/Employment/ACS 2013-2017 Incommute by Industry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11633" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11633" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="8" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="PUMS2013-17 Regional Commuters" sheetId="4" r:id="rId5"/>
     <sheet name="Wrkrs at work vs reg wrkrs" sheetId="6" r:id="rId6"/>
     <sheet name="Ind_Incommute_Values" sheetId="7" r:id="rId7"/>
+    <sheet name="Incommute_Total" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="525">
   <si>
     <t>GEO.id</t>
   </si>
@@ -1597,6 +1598,9 @@
   </si>
   <si>
     <t>in_retempn</t>
+  </si>
+  <si>
+    <t>Incommute_Total</t>
   </si>
 </sst>
 </file>
@@ -10765,7 +10769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B31" sqref="B31:H40"/>
     </sheetView>
   </sheetViews>
@@ -11846,7 +11850,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11903,4 +11907,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>203196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>